<commit_message>
z-score + postive and negative correlations scatterplot (significant)
</commit_message>
<xml_diff>
--- a/HRDH/HRDH_LAB_DATA.xlsx
+++ b/HRDH/HRDH_LAB_DATA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alghziy\colab\HRDH\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alghziy\Desktop\Analysis\colab\HRDH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6971FD-2AC2-4276-A983-4E43CA672A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA88952-EAEA-4F01-A867-A5FDFE756576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" tabRatio="578" activeTab="5" xr2:uid="{99B432AA-E7FF-4414-9695-93001973B8EF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="578" activeTab="1" xr2:uid="{99B432AA-E7FF-4414-9695-93001973B8EF}"/>
   </bookViews>
   <sheets>
     <sheet name="HRDH_697" sheetId="1" r:id="rId1"/>
@@ -374,7 +374,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -571,6 +571,9 @@
     </xf>
     <xf numFmtId="2" fontId="6" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -915,43 +918,43 @@
       <selection pane="bottomRight" activeCell="U15" sqref="U15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="10.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="2"/>
-    <col min="2" max="2" width="7.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="2"/>
+    <col min="2" max="2" width="7.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="9.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="23" max="24" width="5" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="5.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="5.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="5" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="6.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="5.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="5.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="5.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="5.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="34" max="16384" width="8.85546875" style="2"/>
+    <col min="27" max="27" width="5.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="5.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="6.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="5.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="5.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="5.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="5.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="34" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1052,7 +1055,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:33" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:33" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13">
         <v>2</v>
       </c>
@@ -1153,7 +1156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:33" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:33" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
         <v>3</v>
       </c>
@@ -1254,7 +1257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:33" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:33" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
         <v>4</v>
       </c>
@@ -1355,7 +1358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:33" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:33" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <v>5</v>
       </c>
@@ -1456,7 +1459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:33" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:33" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>6</v>
       </c>
@@ -1557,7 +1560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:33" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:33" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>7</v>
       </c>
@@ -1658,7 +1661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:33" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:33" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>8</v>
       </c>
@@ -1759,7 +1762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:33" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:33" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <v>14</v>
       </c>
@@ -1860,7 +1863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:33" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:33" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <v>15</v>
       </c>
@@ -1961,7 +1964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:33" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:33" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13">
         <v>17</v>
       </c>
@@ -2062,19 +2065,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B14" s="4"/>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B15" s="4"/>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B16" s="4"/>
     </row>
   </sheetData>
@@ -2085,53 +2088,53 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13251DC4-F643-4B8F-BBE2-99D95543CC39}">
-  <dimension ref="A1:AH10"/>
+  <dimension ref="A1:AI10"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="S14" sqref="S14"/>
+      <selection pane="bottomRight" activeCell="X18" sqref="X18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="10.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="9.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.88671875" style="5" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="8" style="5" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.88671875" style="5" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="6" style="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="5.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="24" max="25" width="5" style="5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="5.5546875" style="5" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="5" style="5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="5.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="5.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="5.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="35" max="16384" width="8.85546875" style="5"/>
+    <col min="28" max="28" width="5.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="5.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="5.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="5.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="5.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="35" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2235,7 +2238,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:34" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:35" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13">
         <v>17</v>
       </c>
@@ -2338,8 +2341,9 @@
       <c r="AH2" s="55">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:34" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AI2" s="69"/>
+    </row>
+    <row r="3" spans="1:35" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>19</v>
       </c>
@@ -2442,8 +2446,9 @@
       <c r="AH3" s="55">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:34" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AI3" s="69"/>
+    </row>
+    <row r="4" spans="1:35" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <v>20</v>
       </c>
@@ -2546,8 +2551,9 @@
       <c r="AH4" s="55">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:34" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AI4" s="69"/>
+    </row>
+    <row r="5" spans="1:35" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <v>21</v>
       </c>
@@ -2650,8 +2656,9 @@
       <c r="AH5" s="55">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:34" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AI5" s="69"/>
+    </row>
+    <row r="6" spans="1:35" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>61</v>
       </c>
@@ -2754,8 +2761,9 @@
       <c r="AH6" s="55">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:34" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AI6" s="69"/>
+    </row>
+    <row r="7" spans="1:35" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>62</v>
       </c>
@@ -2858,8 +2866,9 @@
       <c r="AH7" s="55">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:34" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AI7" s="69"/>
+    </row>
+    <row r="8" spans="1:35" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>114</v>
       </c>
@@ -2962,8 +2971,9 @@
       <c r="AH8" s="55">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:34" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AI8" s="69"/>
+    </row>
+    <row r="9" spans="1:35" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <v>116</v>
       </c>
@@ -3066,8 +3076,9 @@
       <c r="AH9" s="55">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:34" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AI9" s="69"/>
+    </row>
+    <row r="10" spans="1:35" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <v>126</v>
       </c>
@@ -3170,6 +3181,7 @@
       <c r="AH10" s="55">
         <v>0</v>
       </c>
+      <c r="AI10" s="69"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3187,42 +3199,42 @@
       <selection pane="bottomRight" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="5.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="5.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="16384" width="8.85546875" style="1"/>
+    <col min="27" max="27" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="5.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="6.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="5.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="5.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="5.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="2" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" s="2" customFormat="1" ht="10.8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3323,7 +3335,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>20</v>
       </c>
@@ -3424,7 +3436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <v>21</v>
       </c>
@@ -3525,7 +3537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>22</v>
       </c>
@@ -3626,7 +3638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>23</v>
       </c>
@@ -3727,7 +3739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>24</v>
       </c>
@@ -3828,7 +3840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>36</v>
       </c>
@@ -3929,7 +3941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>37</v>
       </c>
@@ -4030,7 +4042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>38</v>
       </c>
@@ -4131,7 +4143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <v>43</v>
       </c>
@@ -4232,7 +4244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>45</v>
       </c>
@@ -4333,7 +4345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>46</v>
       </c>
@@ -4434,7 +4446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>61</v>
       </c>
@@ -4535,7 +4547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>64</v>
       </c>
@@ -4636,7 +4648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>70</v>
       </c>
@@ -4737,7 +4749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>71</v>
       </c>
@@ -4838,7 +4850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>124</v>
       </c>
@@ -4939,7 +4951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>125</v>
       </c>
@@ -5040,7 +5052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A19" s="9">
         <v>126</v>
       </c>
@@ -5158,43 +5170,43 @@
       <selection pane="bottomRight" activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" style="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" style="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="11.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="11.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5546875" style="11" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" style="11" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" style="11" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9" style="11" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="5.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="6.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="6.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="5.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="6.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="5.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="6.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.33203125" style="11" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="6" style="11" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="6.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="6.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="34" max="16384" width="8.85546875" style="11"/>
+    <col min="32" max="32" width="6.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="6.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="34" max="16384" width="8.88671875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -5295,7 +5307,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="27">
         <v>13</v>
       </c>
@@ -5396,7 +5408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="27">
         <v>14</v>
       </c>
@@ -5497,7 +5509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="27">
         <v>15</v>
       </c>
@@ -5598,7 +5610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="27">
         <v>28</v>
       </c>
@@ -5699,7 +5711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="27">
         <v>29</v>
       </c>
@@ -5800,7 +5812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="27">
         <v>30</v>
       </c>
@@ -5901,7 +5913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="27">
         <v>31</v>
       </c>
@@ -6002,7 +6014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="27">
         <v>51</v>
       </c>
@@ -6103,7 +6115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="27">
         <v>53</v>
       </c>
@@ -6204,7 +6216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="27">
         <v>54</v>
       </c>
@@ -6305,7 +6317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="27">
         <v>55</v>
       </c>
@@ -6406,7 +6418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="27">
         <v>64</v>
       </c>
@@ -6507,7 +6519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="27">
         <v>65</v>
       </c>
@@ -6608,7 +6620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="27">
         <v>68</v>
       </c>
@@ -6709,7 +6721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="27">
         <v>69</v>
       </c>
@@ -6810,7 +6822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="27">
         <v>70</v>
       </c>
@@ -6911,7 +6923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="27">
         <v>92</v>
       </c>
@@ -7012,7 +7024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="27">
         <v>93</v>
       </c>
@@ -7113,7 +7125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="27">
         <v>94</v>
       </c>
@@ -7214,7 +7226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="27">
         <v>95</v>
       </c>
@@ -7315,7 +7327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="27">
         <v>96</v>
       </c>
@@ -7416,7 +7428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="27">
         <v>118</v>
       </c>
@@ -7517,7 +7529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="27">
         <v>119</v>
       </c>
@@ -7618,7 +7630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="27">
         <v>120</v>
       </c>
@@ -7719,7 +7731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="27">
         <v>121</v>
       </c>
@@ -7820,7 +7832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:33" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="27">
         <v>122</v>
       </c>
@@ -7937,43 +7949,43 @@
       <selection pane="bottomRight" activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="10.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" style="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="9.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.44140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.44140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="9.88671875" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.44140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.44140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.88671875" style="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.88671875" style="10" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10" style="10" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.88671875" style="10" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="6" style="10" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.44140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.5546875" style="10" bestFit="1" customWidth="1"/>
     <col min="23" max="24" width="5" style="10" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="5.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="5.5546875" style="10" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="5" style="10" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="5.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="6.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="5.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="5.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="5.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="5.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="34" max="16384" width="8.85546875" style="10"/>
+    <col min="27" max="27" width="5.88671875" style="10" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="5.109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="6.109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="5.5546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="5.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="5.44140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="5.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="34" max="16384" width="8.88671875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -8074,7 +8086,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15">
         <v>15</v>
       </c>
@@ -8175,7 +8187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>16</v>
       </c>
@@ -8276,7 +8288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <v>20</v>
       </c>
@@ -8377,7 +8389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>22</v>
       </c>
@@ -8478,7 +8490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>23</v>
       </c>
@@ -8579,7 +8591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>24</v>
       </c>
@@ -8680,7 +8692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>64</v>
       </c>
@@ -8781,7 +8793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <v>66</v>
       </c>
@@ -8882,7 +8894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <v>67</v>
       </c>
@@ -8983,7 +8995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <v>68</v>
       </c>
@@ -9084,7 +9096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <v>84</v>
       </c>
@@ -9185,7 +9197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
         <v>85</v>
       </c>
@@ -9286,7 +9298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <v>101</v>
       </c>
@@ -9387,7 +9399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <v>102</v>
       </c>
@@ -9488,7 +9500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <v>103</v>
       </c>
@@ -9589,7 +9601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <v>105</v>
       </c>
@@ -9690,7 +9702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <v>128</v>
       </c>
@@ -9791,7 +9803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <v>129</v>
       </c>
@@ -9892,7 +9904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <v>130</v>
       </c>
@@ -9993,7 +10005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <v>144</v>
       </c>
@@ -10094,7 +10106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <v>145</v>
       </c>
@@ -10195,7 +10207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <v>146</v>
       </c>
@@ -10296,7 +10308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <v>147</v>
       </c>
@@ -10397,7 +10409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <v>148</v>
       </c>
@@ -10498,18 +10510,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:33" ht="14.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B32" s="18"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="14"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="14"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="14"/>
     </row>
   </sheetData>
@@ -10521,40 +10533,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FFAF310-B464-43A8-A169-CA4967D58834}">
   <dimension ref="A1:U42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C37" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" style="19" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.33203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" style="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.44140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.33203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.88671875" style="19" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.88671875" style="19" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.88671875" style="19" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" style="19" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.42578125" style="19" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.44140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.33203125" style="19" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="8" style="19" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="22" max="33" width="5.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="34" max="16384" width="8.85546875" style="19"/>
+    <col min="21" max="21" width="11.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="22" max="33" width="5.109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="34" max="16384" width="8.88671875" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -10619,7 +10631,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A2" s="22">
         <v>1</v>
       </c>
@@ -10684,7 +10696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A3" s="21">
         <v>2</v>
       </c>
@@ -10749,7 +10761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A4" s="21">
         <v>3</v>
       </c>
@@ -10814,7 +10826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A5" s="21">
         <v>4</v>
       </c>
@@ -10879,7 +10891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A6" s="21">
         <v>5</v>
       </c>
@@ -10944,7 +10956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A7" s="21">
         <v>6</v>
       </c>
@@ -11009,7 +11021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A8" s="21">
         <v>7</v>
       </c>
@@ -11074,7 +11086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A9" s="21">
         <v>8</v>
       </c>
@@ -11139,7 +11151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A10" s="21">
         <v>9</v>
       </c>
@@ -11204,7 +11216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A11" s="21">
         <v>10</v>
       </c>
@@ -11269,7 +11281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A12" s="22">
         <v>11</v>
       </c>
@@ -11334,7 +11346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A13" s="22">
         <v>12</v>
       </c>
@@ -11399,7 +11411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A14" s="22">
         <v>13</v>
       </c>
@@ -11464,7 +11476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A15" s="22">
         <v>14</v>
       </c>
@@ -11529,7 +11541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A16" s="22">
         <v>15</v>
       </c>
@@ -11594,7 +11606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A17" s="22">
         <v>16</v>
       </c>
@@ -11659,7 +11671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A18" s="22">
         <v>17</v>
       </c>
@@ -11724,7 +11736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A19" s="22">
         <v>18</v>
       </c>
@@ -11789,7 +11801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A20" s="22">
         <v>19</v>
       </c>
@@ -11854,7 +11866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:21" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A21" s="22">
         <v>20</v>
       </c>
@@ -11919,7 +11931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="22">
         <v>21</v>
       </c>
@@ -11984,7 +11996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:21" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A23" s="22">
         <v>22</v>
       </c>
@@ -12049,7 +12061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="22">
         <v>23</v>
       </c>
@@ -12114,7 +12126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A25" s="22">
         <v>24</v>
       </c>
@@ -12179,7 +12191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A26" s="22">
         <v>25</v>
       </c>
@@ -12244,7 +12256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A27" s="22">
         <v>26</v>
       </c>
@@ -12309,7 +12321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:21" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A28" s="22">
         <v>27</v>
       </c>
@@ -12374,7 +12386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A29" s="22">
         <v>28</v>
       </c>
@@ -12439,7 +12451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:21" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A30" s="22">
         <v>29</v>
       </c>
@@ -12504,7 +12516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:21" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A31" s="22">
         <v>30</v>
       </c>
@@ -12569,7 +12581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:21" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A32" s="22">
         <v>31</v>
       </c>
@@ -12634,7 +12646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:21" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A33" s="22">
         <v>32</v>
       </c>
@@ -12699,7 +12711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:21" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A34" s="22">
         <v>33</v>
       </c>
@@ -12764,7 +12776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:21" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A35" s="22">
         <v>34</v>
       </c>
@@ -12829,7 +12841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:21" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A36" s="22">
         <v>35</v>
       </c>
@@ -12894,7 +12906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:21" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A37" s="22">
         <v>36</v>
       </c>
@@ -12959,7 +12971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:21" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A38" s="22">
         <v>37</v>
       </c>
@@ -13024,7 +13036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:21" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A39" s="22">
         <v>38</v>
       </c>
@@ -13089,7 +13101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:21" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A40" s="22">
         <v>39</v>
       </c>
@@ -13154,7 +13166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:21" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A41" s="22">
         <v>40</v>
       </c>
@@ -13219,7 +13231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:21" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A42" s="43">
         <v>41</v>
       </c>
@@ -13300,34 +13312,34 @@
       <selection pane="bottomRight" activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" style="19" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" style="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" style="19" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="19" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" style="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.88671875" style="19" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.33203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.33203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.109375" style="19" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10" style="19" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.33203125" style="19" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10" style="19" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="7" style="19" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.42578125" style="19" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="8.85546875" style="19"/>
+    <col min="21" max="21" width="8.44140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="8.88671875" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -13395,7 +13407,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="23">
         <v>1</v>
       </c>
@@ -13464,7 +13476,7 @@
       </c>
       <c r="W2" s="22"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="23">
         <v>2</v>
       </c>
@@ -13533,7 +13545,7 @@
       </c>
       <c r="W3" s="22"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="23">
         <v>3</v>
       </c>
@@ -13602,7 +13614,7 @@
       </c>
       <c r="W4" s="22"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="23">
         <v>4</v>
       </c>
@@ -13671,7 +13683,7 @@
       </c>
       <c r="W5" s="22"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="23">
         <v>5</v>
       </c>
@@ -13740,7 +13752,7 @@
       </c>
       <c r="W6" s="22"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="23">
         <v>6</v>
       </c>
@@ -13809,7 +13821,7 @@
       </c>
       <c r="W7" s="22"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="23">
         <v>7</v>
       </c>
@@ -13878,7 +13890,7 @@
       </c>
       <c r="W8" s="22"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="23">
         <v>8</v>
       </c>
@@ -13947,7 +13959,7 @@
       </c>
       <c r="W9" s="22"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="23">
         <v>9</v>
       </c>
@@ -14016,7 +14028,7 @@
       </c>
       <c r="W10" s="22"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="23">
         <v>10</v>
       </c>
@@ -14085,7 +14097,7 @@
       </c>
       <c r="W11" s="22"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="23">
         <v>11</v>
       </c>
@@ -14154,7 +14166,7 @@
       </c>
       <c r="W12" s="22"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="23">
         <v>12</v>
       </c>
@@ -14223,7 +14235,7 @@
       </c>
       <c r="W13" s="22"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="23">
         <v>13</v>
       </c>
@@ -14292,7 +14304,7 @@
       </c>
       <c r="W14" s="22"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="23">
         <v>14</v>
       </c>
@@ -14361,7 +14373,7 @@
       </c>
       <c r="W15" s="22"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="23">
         <v>15</v>
       </c>
@@ -14430,7 +14442,7 @@
       </c>
       <c r="W16" s="22"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="23">
         <v>16</v>
       </c>
@@ -14499,7 +14511,7 @@
       </c>
       <c r="W17" s="22"/>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="23">
         <v>17</v>
       </c>
@@ -14568,7 +14580,7 @@
       </c>
       <c r="W18" s="22"/>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="23">
         <v>18</v>
       </c>
@@ -14637,7 +14649,7 @@
       </c>
       <c r="W19" s="22"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="23">
         <v>19</v>
       </c>
@@ -14706,7 +14718,7 @@
       </c>
       <c r="W20" s="22"/>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="23">
         <v>20</v>
       </c>
@@ -14775,7 +14787,7 @@
       </c>
       <c r="W21" s="22"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="23">
         <v>21</v>
       </c>

</xml_diff>